<commit_message>
added course grade as cirteria
</commit_message>
<xml_diff>
--- a/src/allotment.xlsx
+++ b/src/allotment.xlsx
@@ -397,306 +397,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AV2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>EEL2020</v>
+        <v>eel1010</v>
       </c>
       <c r="B1" t="str">
-        <v>EEL3080</v>
-      </c>
-      <c r="C1" t="str">
-        <v>EEL7150</v>
-      </c>
-      <c r="D1" t="str">
-        <v>EEL3090</v>
-      </c>
-      <c r="E1" t="str">
-        <v>EEL3100</v>
-      </c>
-      <c r="F1" t="str">
-        <v>EEL2050</v>
-      </c>
-      <c r="G1" t="str">
-        <v>SHL7430</v>
-      </c>
-      <c r="H1" t="str">
-        <v>EEL3060</v>
-      </c>
-      <c r="I1" t="str">
-        <v>EEL2040</v>
-      </c>
-      <c r="J1" t="str">
-        <v>EEL7260</v>
-      </c>
-      <c r="K1" t="str">
-        <v>EEL2030</v>
-      </c>
-      <c r="L1" t="str">
-        <v>EEL1000</v>
-      </c>
-      <c r="M1" t="str">
-        <v>EEL2010</v>
-      </c>
-      <c r="N1" t="str">
-        <v>EEL7130</v>
-      </c>
-      <c r="O1" t="str">
-        <v>EEL3070</v>
-      </c>
-      <c r="P1" t="str">
-        <v>csl1011</v>
-      </c>
-      <c r="Q1" t="str">
-        <v>csl1013</v>
-      </c>
-      <c r="R1" t="str">
-        <v>EEL7650</v>
-      </c>
-      <c r="S1" t="str">
-        <v>csl1012</v>
-      </c>
-      <c r="T1" t="str">
-        <v>csl1018</v>
-      </c>
-      <c r="U1" t="str">
-        <v>csl1016</v>
-      </c>
-      <c r="V1" t="str">
-        <v>csl1014</v>
-      </c>
-      <c r="W1" t="str">
-        <v>csl1015</v>
-      </c>
-      <c r="X1" t="str">
-        <v>EEL7480</v>
-      </c>
-      <c r="Y1" t="str">
-        <v>csl1017</v>
-      </c>
-      <c r="Z1" t="str">
-        <v>csl1019</v>
-      </c>
-      <c r="AA1" t="str">
-        <v>csl1111</v>
-      </c>
-      <c r="AB1" t="str">
-        <v>EEL1111</v>
-      </c>
-      <c r="AC1" t="str">
-        <v>eel2020</v>
-      </c>
-      <c r="AD1" t="str">
-        <v>eel7260</v>
-      </c>
-      <c r="AE1" t="str">
-        <v>B20CS002</v>
-      </c>
-      <c r="AF1" t="str">
-        <v>B20CS003</v>
-      </c>
-      <c r="AG1" t="str">
-        <v>B20CS001</v>
-      </c>
-      <c r="AH1" t="str">
-        <v>B20CS004</v>
-      </c>
-      <c r="AI1" t="str">
-        <v>B20CS007</v>
-      </c>
-      <c r="AJ1" t="str">
-        <v>B20CS107</v>
-      </c>
-      <c r="AK1" t="str">
-        <v>B20CS008</v>
-      </c>
-      <c r="AL1" t="str">
-        <v>B20CS006</v>
-      </c>
-      <c r="AM1" t="str">
-        <v>B20CS009</v>
-      </c>
-      <c r="AN1" t="str">
-        <v>B20EE099</v>
-      </c>
-      <c r="AO1" t="str">
-        <v>B20CS097</v>
-      </c>
-      <c r="AP1" t="str">
-        <v>B20CS109</v>
-      </c>
-      <c r="AQ1" t="str">
-        <v>B20CS029</v>
-      </c>
-      <c r="AR1" t="str">
-        <v>B20CS110</v>
-      </c>
-      <c r="AS1" t="str">
-        <v>b20cs067</v>
-      </c>
-      <c r="AT1" t="str">
-        <v>b20cs019</v>
-      </c>
-      <c r="AU1" t="str">
-        <v>b20cs006</v>
-      </c>
-      <c r="AV1" t="str">
-        <v>b20cs008</v>
+        <v>b20ee011</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>B20CS001,B20CS097,b20cs019</v>
+        <v>b20ee011</v>
       </c>
       <c r="B2" t="str">
-        <v>B20CS007,B20CS097,b20cs006</v>
-      </c>
-      <c r="C2" t="str">
-        <v>B20CS004,B20CS109,b20cs006</v>
-      </c>
-      <c r="D2" t="str">
-        <v>B20CS001,B20CS109,b20cs006</v>
-      </c>
-      <c r="E2" t="str">
-        <v>B20CS003,B20CS109,b20cs008</v>
-      </c>
-      <c r="F2" t="str">
-        <v>B20CS004,B20CS029,b20cs008</v>
-      </c>
-      <c r="G2" t="str">
-        <v>B20CS004</v>
-      </c>
-      <c r="H2" t="str">
-        <v>B20CS003,B20CS029,b20cs008</v>
-      </c>
-      <c r="I2" t="str">
-        <v>B20CS007,B20CS029</v>
-      </c>
-      <c r="J2" t="str">
-        <v>B20CS009</v>
-      </c>
-      <c r="K2" t="str">
-        <v>B20CS003,B20CS110</v>
-      </c>
-      <c r="L2" t="str">
-        <v>B20CS009,B20EE099,B20CS110</v>
-      </c>
-      <c r="M2" t="str">
-        <v>B20CS001,B20CS110</v>
-      </c>
-      <c r="N2" t="str">
-        <v>B20CS002</v>
-      </c>
-      <c r="O2" t="str">
-        <v>B20CS009,b20cs067</v>
-      </c>
-      <c r="P2" t="str">
-        <v>B20CS002</v>
-      </c>
-      <c r="Q2" t="str">
-        <v>B20CS002</v>
-      </c>
-      <c r="R2" t="str">
-        <v>B20CS007,b20cs067</v>
-      </c>
-      <c r="S2" t="str">
-        <v>B20CS107</v>
-      </c>
-      <c r="T2" t="str">
-        <v>B20CS107</v>
-      </c>
-      <c r="U2" t="str">
-        <v>B20CS107</v>
-      </c>
-      <c r="V2" t="str">
-        <v>B20CS008</v>
-      </c>
-      <c r="W2" t="str">
-        <v>B20CS008</v>
-      </c>
-      <c r="X2" t="str">
-        <v>B20CS006</v>
-      </c>
-      <c r="Y2" t="str">
-        <v>B20CS008</v>
-      </c>
-      <c r="Z2" t="str">
-        <v>B20CS006</v>
-      </c>
-      <c r="AA2" t="str">
-        <v>B20CS006</v>
-      </c>
-      <c r="AB2" t="str">
-        <v>B20EE099,b20cs067</v>
-      </c>
-      <c r="AC2" t="str">
-        <v>B20EE099,b20cs019</v>
-      </c>
-      <c r="AD2" t="str">
-        <v>B20CS097,b20cs019</v>
-      </c>
-      <c r="AE2" t="str">
-        <v>EEL7130,csl1011,csl1013</v>
-      </c>
-      <c r="AF2" t="str">
-        <v>EEL3100,EEL3060,EEL2030</v>
-      </c>
-      <c r="AG2" t="str">
-        <v>EEL2020,EEL3090,EEL2010</v>
-      </c>
-      <c r="AH2" t="str">
-        <v>EEL7150,EEL2050,SHL7430</v>
-      </c>
-      <c r="AI2" t="str">
-        <v>EEL3080,EEL2040,EEL7650</v>
-      </c>
-      <c r="AJ2" t="str">
-        <v>csl1012,csl1018,csl1016</v>
-      </c>
-      <c r="AK2" t="str">
-        <v>csl1014,csl1015,csl1017</v>
-      </c>
-      <c r="AL2" t="str">
-        <v>EEL7480,csl1019,csl1111</v>
-      </c>
-      <c r="AM2" t="str">
-        <v>EEL7260,EEL1000,EEL3070</v>
-      </c>
-      <c r="AN2" t="str">
-        <v>EEL1000,EEL1111,eel2020</v>
-      </c>
-      <c r="AO2" t="str">
-        <v>eel7260,EEL2020,EEL3080</v>
-      </c>
-      <c r="AP2" t="str">
-        <v>EEL7150,EEL3090,EEL3100</v>
-      </c>
-      <c r="AQ2" t="str">
-        <v>EEL2050,EEL3060,EEL2040</v>
-      </c>
-      <c r="AR2" t="str">
-        <v>EEL2030,EEL1000,EEL2010</v>
-      </c>
-      <c r="AS2" t="str">
-        <v>EEL3070,EEL7650,EEL1111</v>
-      </c>
-      <c r="AT2" t="str">
-        <v>eel2020,eel7260,EEL2020</v>
-      </c>
-      <c r="AU2" t="str">
-        <v>EEL3080,EEL7150,EEL3090</v>
-      </c>
-      <c r="AV2" t="str">
-        <v>EEL3100,EEL2050,EEL3060</v>
+        <v>eel1010</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AV2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added cgpa and weight
</commit_message>
<xml_diff>
--- a/src/allotment.xlsx
+++ b/src/allotment.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>course Code</t>
   </si>
@@ -22,16 +22,7 @@
     <t>EEL1010</t>
   </si>
   <si>
-    <t>B20EE0124</t>
-  </si>
-  <si>
     <t>B20EE011</t>
-  </si>
-  <si>
-    <t>CSL1010</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -408,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -419,23 +410,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>